<commit_message>
feat(inheritance): added Address, Company, Employee, and test classes chore(inheritance): updated Customer and Tester implementations docs: updated classNotes.xlsx and added inheritance explanation doc
</commit_message>
<xml_diff>
--- a/material/classNotes.xlsx
+++ b/material/classNotes.xlsx
@@ -10,7 +10,10 @@
     <sheet name="Class, Object, Constructor" sheetId="1" r:id="rId1"/>
     <sheet name="Encapsulation" sheetId="2" r:id="rId2"/>
     <sheet name="Inheritance" sheetId="3" r:id="rId3"/>
-    <sheet name="Polymorphism" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId4"/>
+    <sheet name="Polymorphism" sheetId="4" r:id="rId5"/>
+    <sheet name="Abstraction" sheetId="5" r:id="rId6"/>
+    <sheet name="Exception Handling" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="232">
   <si>
     <t>CLASS</t>
   </si>
@@ -276,32 +279,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>refer to the current object</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">We want to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>call another constructor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from a constructor</t>
     </r>
   </si>
   <si>
@@ -694,9 +671,6 @@
     <t>AGGREGATION</t>
   </si>
   <si>
-    <t xml:space="preserve"> - one class contains another class as a field</t>
-  </si>
-  <si>
     <r>
       <t>Inheritance (</t>
     </r>
@@ -1209,6 +1183,59 @@
     </r>
   </si>
   <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Close Friends</t>
+  </si>
+  <si>
+    <t>Outsiders</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>guestHouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Data Hiding</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We want to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>call another constructor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from a constructor in the same class</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve"> - shared across all objects
 - it belongs to the </t>
@@ -1233,42 +1260,724 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> instead of any individual object.
- - memory allocated only once</t>
-    </r>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>Close Friends</t>
-  </si>
-  <si>
-    <t>Outsiders</t>
-  </si>
-  <si>
-    <t>mobile</t>
-  </si>
-  <si>
-    <t>house</t>
-  </si>
-  <si>
-    <t>car</t>
-  </si>
-  <si>
-    <t>guestHouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Data Hiding</t>
+ - memory allocated only once
+ - memory allocated when the class is loaded</t>
+    </r>
+  </si>
+  <si>
+    <t>ABSTRACTION</t>
+  </si>
+  <si>
+    <r>
+      <t>Abstraction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the process of hiding internal details and showing only the essential features.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Think of it like </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>using a TV remote</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You press a button, and it works — you don't need to know </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>how</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the signal reaches the TV or how circuits work inside. That’s abstraction!</t>
+    </r>
+  </si>
+  <si>
+    <t>ABSTRACT CLASS</t>
+  </si>
+  <si>
+    <t>Rules:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Declared using the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>abstract</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keyword.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cannot be instantiated</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (you cannot create an object of an abstract class).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Can have </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>abstract methods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (without body) and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concrete methods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (with body).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Used as a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>base class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to be extended by subclasses.</t>
+    </r>
+  </si>
+  <si>
+    <t>Abstract Class</t>
+  </si>
+  <si>
+    <t>Can have constructors?</t>
+  </si>
+  <si>
+    <t>Can have abstract methods?</t>
+  </si>
+  <si>
+    <t>Can have non-abstract methods?</t>
+  </si>
+  <si>
+    <t>Can be instantiated?</t>
+  </si>
+  <si>
+    <t>Can have variables?</t>
+  </si>
+  <si>
+    <t>Supports inheritance?</t>
+  </si>
+  <si>
+    <t>INTERFACE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interface</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100% abstract blueprint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of a class.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It contains </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>only method declarations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (until Java 7), and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no method bodies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (implementation).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It tells </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>what to do</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, but </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not how to do it</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — like a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contract</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that any class implementing it must follow.</t>
+    </r>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>✅ Yes (by default)</t>
+  </si>
+  <si>
+    <t>Can have method bodies?</t>
+  </si>
+  <si>
+    <t>❌ No (until Java 7)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">✅ Yes, but must be </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>public static final</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (constants)</t>
+    </r>
+  </si>
+  <si>
+    <t>Can extend another interface?</t>
+  </si>
+  <si>
+    <t>Can a class implement multiple interfaces?</t>
+  </si>
+  <si>
+    <t>✅ Yes (supports multiple inheritance)</t>
+  </si>
+  <si>
+    <t>Can interfaces have constructors?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Java 8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> onwards
+Interfaces can have:
+default methods (with body)
+static methods</t>
+    </r>
+  </si>
+  <si>
+    <t>Default implementation</t>
+  </si>
+  <si>
+    <t>❌ (until Java 8)</t>
+  </si>
+  <si>
+    <t>✅</t>
+  </si>
+  <si>
+    <t>Multiple inheritance</t>
+  </si>
+  <si>
+    <t>✅ (via multiple interfaces)</t>
+  </si>
+  <si>
+    <t>❌</t>
+  </si>
+  <si>
+    <t>Constructor allowed</t>
+  </si>
+  <si>
+    <t>Can have fields</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Only </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>public static final</t>
+    </r>
+  </si>
+  <si>
+    <t>Any access modifiers</t>
+  </si>
+  <si>
+    <t>EXCEPTION HANDLING</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exception</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unexpected event</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that occurs during program execution and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>disrupts the normal flow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of instructions.</t>
+    </r>
+  </si>
+  <si>
+    <t>Handled By</t>
+  </si>
+  <si>
+    <t>Checked Exception</t>
+  </si>
+  <si>
+    <t>FileNotFoundException, IOException</t>
+  </si>
+  <si>
+    <t>Compiler forces handling</t>
+  </si>
+  <si>
+    <t>Unchecked Exception</t>
+  </si>
+  <si>
+    <t>ArithmeticException, NullPointerException</t>
+  </si>
+  <si>
+    <t>Not checked at compile-time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try {
+    // risky code
+} catch(ExceptionType e) {
+    // handling code
+} finally {
+    // (optional) code that always executes
+}
+</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>ArithmeticException</t>
+  </si>
+  <si>
+    <t>Divide by zero</t>
+  </si>
+  <si>
+    <t>NullPointerException</t>
+  </si>
+  <si>
+    <t>Using object without initialization</t>
+  </si>
+  <si>
+    <t>ArrayIndexOutOfBoundsException</t>
+  </si>
+  <si>
+    <t>Invalid array index</t>
+  </si>
+  <si>
+    <t>NumberFormatException</t>
+  </si>
+  <si>
+    <t>Invalid string to number conversion</t>
+  </si>
+  <si>
+    <t>ClassNotFoundException</t>
+  </si>
+  <si>
+    <t>Class not found during loading</t>
+  </si>
+  <si>
+    <t>IOException</t>
+  </si>
+  <si>
+    <t>Input/Output failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try {
+    // code
+} catch (ArithmeticException e) {
+    // handle ArithmeticException
+} catch (ArrayIndexOutOfBoundsException e) {
+    // handle Array issue
+} catch (Exception e) {
+    // general catch
+}
+</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>throw</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Used to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>throw an exception manually</t>
+    </r>
+  </si>
+  <si>
+    <t>throws</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Declares </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that a method might throw</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> exception</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - one class contains another class as a field(property - instance var)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - child class constructor will always call parent class default constructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - super keyword points the immediate parent</t>
+  </si>
+  <si>
+    <t>https://github.com/fresher2coder/sret-java-bsc-26.git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1348,6 +2057,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1408,7 +2125,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1464,6 +2181,16 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1471,7 +2198,226 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="59">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1819,81 +2765,149 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C26:E29" totalsRowShown="0" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C26:E29" totalsRowShown="0" headerRowDxfId="58">
   <autoFilter ref="C26:E29"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Concept" dataDxfId="34"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="33"/>
-    <tableColumn id="3" name="Example" dataDxfId="32"/>
+    <tableColumn id="1" name="Concept" dataDxfId="57"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="56"/>
+    <tableColumn id="3" name="Example" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D23:E29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="20">
+  <autoFilter ref="D23:E29"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Feature" dataDxfId="22"/>
+    <tableColumn id="2" name="Abstract Class" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="D41:E47" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+  <autoFilter ref="D41:E47"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Feature" dataDxfId="18"/>
+    <tableColumn id="2" name="Interface" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="D51:F55" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11">
+  <autoFilter ref="D51:F55"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Feature" dataDxfId="14"/>
+    <tableColumn id="2" name="Interface" dataDxfId="13"/>
+    <tableColumn id="3" name="Abstract Class" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="D6:F8" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="D6:F8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Type" dataDxfId="9"/>
+    <tableColumn id="2" name="Example" dataDxfId="8"/>
+    <tableColumn id="3" name="Handled By" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="D10:E16" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="D10:E16"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Exception" dataDxfId="5"/>
+    <tableColumn id="2" name="Description" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="D19:E21" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="D19:E21"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Keyword" dataDxfId="2"/>
+    <tableColumn id="2" name="Purpose" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="D43:E47" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="D43:E47" totalsRowShown="0" headerRowDxfId="54">
   <autoFilter ref="D43:E47"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Usage" dataDxfId="30"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="29"/>
+    <tableColumn id="1" name="Usage" dataDxfId="53"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="D54:E58" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="D54:E58" totalsRowShown="0" headerRowDxfId="51">
   <autoFilter ref="D54:E58"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="What you can mark as static" dataDxfId="27"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="26"/>
+    <tableColumn id="1" name="What you can mark as static" dataDxfId="50"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C62:E66" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C62:E66" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="C62:E66"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Feature" dataDxfId="23"/>
-    <tableColumn id="2" name="Static" dataDxfId="22"/>
-    <tableColumn id="3" name="Non-static (Instance)" dataDxfId="21"/>
+    <tableColumn id="1" name="Feature" dataDxfId="46"/>
+    <tableColumn id="2" name="Static" dataDxfId="45"/>
+    <tableColumn id="3" name="Non-static (Instance)" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="D7:E11" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="D7:E11" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="D7:E11"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Modifier" dataDxfId="19"/>
-    <tableColumn id="2" name="Who Can Access?" dataDxfId="18"/>
+    <tableColumn id="1" name="Modifier" dataDxfId="42"/>
+    <tableColumn id="2" name="Who Can Access?" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D15:H19" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D15:H19" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="D15:H19"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Access Modifier" dataDxfId="15"/>
-    <tableColumn id="2" name="Same Class" dataDxfId="14"/>
-    <tableColumn id="3" name="Same Package" dataDxfId="13"/>
-    <tableColumn id="4" name="Subclass (Other Pkg)" dataDxfId="12"/>
-    <tableColumn id="5" name="Other Pkg" dataDxfId="11"/>
+    <tableColumn id="1" name="Access Modifier" dataDxfId="38"/>
+    <tableColumn id="2" name="Same Class" dataDxfId="37"/>
+    <tableColumn id="3" name="Same Package" dataDxfId="36"/>
+    <tableColumn id="4" name="Subclass (Other Pkg)" dataDxfId="35"/>
+    <tableColumn id="5" name="Other Pkg" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="D29:E32" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="D29:E32" totalsRowShown="0" headerRowDxfId="33">
   <autoFilter ref="D29:E32"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Concept" dataDxfId="9"/>
+    <tableColumn id="1" name="Concept" dataDxfId="32"/>
     <tableColumn id="2" name="Done Using"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1901,24 +2915,24 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="D11:F16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="D11:F16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="D14:F19" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="D14:F19"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Feature" dataDxfId="6"/>
-    <tableColumn id="2" name="Inheritance (is-a)" dataDxfId="5"/>
-    <tableColumn id="3" name="Aggregation (has-a)" dataDxfId="4"/>
+    <tableColumn id="1" name="Feature" dataDxfId="29"/>
+    <tableColumn id="2" name="Inheritance (is-a)" dataDxfId="28"/>
+    <tableColumn id="3" name="Aggregation (has-a)" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="D13:F17" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="D13:F17" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="D13:F17"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Rule" dataDxfId="2"/>
-    <tableColumn id="2" name="Description" dataDxfId="1"/>
-    <tableColumn id="3" name="Example" dataDxfId="0"/>
+    <tableColumn id="1" name="Rule" dataDxfId="25"/>
+    <tableColumn id="2" name="Description" dataDxfId="24"/>
+    <tableColumn id="3" name="Example" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2189,7 +3203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E66"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -2369,7 +3383,7 @@
         <v>3</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>32</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2379,7 +3393,7 @@
     </row>
     <row r="43" spans="1:5">
       <c r="D43" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>17</v>
@@ -2387,49 +3401,49 @@
     </row>
     <row r="44" spans="1:5">
       <c r="D44" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="28.8">
       <c r="D45" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="D46" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="28.8">
       <c r="D47" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="57.6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="72">
       <c r="B53" s="15" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="D54" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>17</v>
@@ -2437,34 +3451,34 @@
     </row>
     <row r="55" spans="2:5">
       <c r="D55" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="56" spans="2:5" ht="28.8">
       <c r="D56" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="57" spans="2:5">
       <c r="D57" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="58" spans="2:5">
       <c r="D58" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="61" spans="2:5">
@@ -2474,18 +3488,18 @@
     </row>
     <row r="62" spans="2:5">
       <c r="C62" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="E62" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="63" spans="2:5">
       <c r="C63" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D63" s="10" t="s">
         <v>18</v>
@@ -2496,35 +3510,35 @@
     </row>
     <row r="64" spans="2:5">
       <c r="C64" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="E64" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="65" spans="3:5">
       <c r="C65" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D65" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="E65" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="66" spans="3:5">
       <c r="C66" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="E66" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2543,8 +3557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2562,173 +3576,173 @@
   <sheetData>
     <row r="3" spans="2:8">
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="57.6">
       <c r="B5" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:8">
       <c r="D6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="D7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="D8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="D9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="28.8">
       <c r="D10" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="28.8">
       <c r="D11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>76</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="E14" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="15" spans="2:8">
       <c r="D15" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="2:8">
       <c r="C16" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>84</v>
-      </c>
       <c r="G16" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="C17" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E17" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="C18" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="2:8">
       <c r="C19" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -2736,17 +3750,17 @@
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="43.2">
       <c r="B25" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="57.6">
       <c r="B27" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="2:8">
@@ -2759,31 +3773,31 @@
         <v>16</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="28.8">
       <c r="D30" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="2:8">
       <c r="D31" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="28.8">
       <c r="D32" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2798,10 +3812,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2817,94 +3831,107 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="28.8">
+      <c r="B6" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="28.8">
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="2:6">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="2:6" ht="28.8">
+      <c r="B8" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="28.8">
+      <c r="B9" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="18" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="18" t="s">
+      <c r="D12" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="28.8">
+      <c r="B14" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="1" t="s">
+      <c r="F14" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="9" t="s">
+    </row>
+    <row r="15" spans="2:6" ht="28.8">
+      <c r="D15" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="E15" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="28.8">
-      <c r="D12" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="10" t="s">
+    </row>
+    <row r="16" spans="2:6">
+      <c r="D16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
-      <c r="D13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="10" t="s">
+    <row r="17" spans="4:6">
+      <c r="D17" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="E17" s="11" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="D14" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="11" t="s">
+    </row>
+    <row r="18" spans="4:6">
+      <c r="D18" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="D15" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="10" t="s">
+    </row>
+    <row r="19" spans="4:6" ht="28.8">
+      <c r="D19" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="28.8">
-      <c r="D16" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>115</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2917,9 +3944,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:3">
+      <c r="C4" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2936,22 +3986,22 @@
   <sheetData>
     <row r="3" spans="2:6">
       <c r="B3" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="43.2">
       <c r="B5" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -2959,13 +4009,13 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>4</v>
@@ -2973,61 +4023,61 @@
     </row>
     <row r="14" spans="2:6" ht="28.8">
       <c r="B14" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="28.8">
       <c r="B15" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="28.8">
       <c r="B16" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="28.8">
       <c r="B17" s="20"/>
       <c r="D17" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -3035,53 +4085,53 @@
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="27.6">
       <c r="B25" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C25" s="21"/>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C26" s="21"/>
     </row>
     <row r="27" spans="2:6" ht="27.6">
       <c r="B27" s="22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C27" s="21"/>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" s="21"/>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C29" s="21"/>
     </row>
     <row r="30" spans="2:6" ht="27.6">
       <c r="B30" s="22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C30" s="21"/>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3090,4 +4140,454 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A47" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="35.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="27.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="43.2">
+      <c r="B5" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="57.6">
+      <c r="B8" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" s="26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" ht="18">
+      <c r="B14" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" s="24"/>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" s="24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="24"/>
+    </row>
+    <row r="18" spans="2:5" ht="28.8">
+      <c r="B18" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="24"/>
+    </row>
+    <row r="20" spans="2:5" ht="28.8">
+      <c r="B20" s="24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="24"/>
+    </row>
+    <row r="22" spans="2:5" ht="28.8">
+      <c r="B22" s="24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="D23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="D24" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="D25" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="28.8">
+      <c r="D26" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="D27" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="D28" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="D29" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="28.8">
+      <c r="B36" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="86.4">
+      <c r="B37" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="2:5" ht="43.2">
+      <c r="B39" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="D41" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="D42" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="D43" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="28.8">
+      <c r="D44" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="D45" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="28.8">
+      <c r="D46" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="28.8">
+      <c r="D47" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" ht="28.8">
+      <c r="D51" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6">
+      <c r="D52" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6">
+      <c r="D53" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6">
+      <c r="D54" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" ht="43.2">
+      <c r="D55" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="35.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6">
+      <c r="B3" s="14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="43.2">
+      <c r="B5" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="D6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="28.8">
+      <c r="D7" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="28.8">
+      <c r="D8" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="115.2">
+      <c r="B9" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="D10" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="D11" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="D12" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="26.4">
+      <c r="D13" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="28.8">
+      <c r="D14" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="26.4">
+      <c r="D15" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="D16" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="158.4">
+      <c r="B18" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="D19" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="28.8">
+      <c r="D20" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="28.8">
+      <c r="D21" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>